<commit_message>
Bring in new data for April 2018
</commit_message>
<xml_diff>
--- a/data/Cam_ElectionSeason.xlsx
+++ b/data/Cam_ElectionSeason.xlsx
@@ -493,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -705,6 +705,22 @@
         <v>0</v>
       </c>
     </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="4">
+        <v>22</v>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>